<commit_message>
feat: Catch dialog and view allow the bot to gracefully handle errors.
</commit_message>
<xml_diff>
--- a/packages/test-complexdialogs/intents.xlsx
+++ b/packages/test-complexdialogs/intents.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="sample-complexdialogs" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
   <si>
     <t xml:space="preserve">alcohol</t>
   </si>
@@ -98,6 +98,51 @@
   </si>
   <si>
     <t xml:space="preserve">I leave from Paris.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">disanbiguationone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">je veux résilier ma seconde carte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">je veux résilier ma carte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">résiliation de ma carte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">comment faire une résiliation ? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">comment puis-je procéder?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">je veux accéder au formulaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">je ne veux plus l'utiliser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">je veux arrêter </t>
+  </si>
+  <si>
+    <t xml:space="preserve">disanbiguationtwo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">je veux boire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">je veux jouer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">je veux manger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i see a disambiguation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">error</t>
   </si>
 </sst>
 </file>
@@ -194,17 +239,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A36"/>
+  <dimension ref="A1:A55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G49" activeCellId="0" sqref="G49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.34"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -347,10 +392,90 @@
         <v>25</v>
       </c>
     </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>